<commit_message>
Performed calibration of the needle
Signed-off-by: Dimitri Lezcano <dlezcan1@jhu.edu>
</commit_message>
<xml_diff>
--- a/FBG_Needle_Calibration_Data/needle_1/Calibration/0 deg/12-28-19_14-41/curvature_data.xlsx
+++ b/FBG_Needle_Calibration_Data/needle_1/Calibration/0 deg/12-28-19_14-41/curvature_data.xlsx
@@ -379,44 +379,44 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>52963.406994</v>
+        <v>52899.342991</v>
       </c>
       <c r="B2">
-        <v>-0.00018641813817</v>
+        <v>-3.942213424e-05</v>
       </c>
       <c r="C2">
-        <v>-0.00015060479696</v>
+        <v>-3.0275960474e-05</v>
       </c>
       <c r="D2">
-        <v>-4.4232515122e-05</v>
+        <v>-3.2085221738e-06</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>52973.938995</v>
+        <v>52922.142992</v>
       </c>
       <c r="B3">
-        <v>-3.2965453674e-05</v>
+        <v>-0.00020350871801</v>
       </c>
       <c r="C3">
-        <v>-2.6705059835e-05</v>
+        <v>-0.0001621936335</v>
       </c>
       <c r="D3">
-        <v>-8.1586853441e-06</v>
+        <v>-3.9442408426e-05</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>52953.142994</v>
+        <v>52933.142993</v>
       </c>
       <c r="B4">
-        <v>-0.0004484188</v>
+        <v>-0.00046556799422</v>
       </c>
       <c r="C4">
-        <v>-0.0003643707</v>
+        <v>-0.00037468526522</v>
       </c>
       <c r="D4">
-        <v>-0.000104648</v>
+        <v>-9.4001703476e-05</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -435,44 +435,44 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
-        <v>52922.142992</v>
+        <v>52953.142994</v>
       </c>
       <c r="B6">
-        <v>-0.00020350871801</v>
+        <v>-0.0004484188</v>
       </c>
       <c r="C6">
-        <v>-0.0001621936335</v>
+        <v>-0.0003643707</v>
       </c>
       <c r="D6">
-        <v>-3.9442408426e-05</v>
+        <v>-0.000104648</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>52933.142993</v>
+        <v>52963.406994</v>
       </c>
       <c r="B7">
-        <v>-0.00046556799422</v>
+        <v>-0.00018641813817</v>
       </c>
       <c r="C7">
-        <v>-0.00037468526522</v>
+        <v>-0.00015060479696</v>
       </c>
       <c r="D7">
-        <v>-9.4001703476e-05</v>
+        <v>-4.4232515122e-05</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>52899.342991</v>
+        <v>52973.938995</v>
       </c>
       <c r="B8">
-        <v>-3.942213424e-05</v>
+        <v>-3.2965453674e-05</v>
       </c>
       <c r="C8">
-        <v>-3.0275960474e-05</v>
+        <v>-2.6705059835e-05</v>
       </c>
       <c r="D8">
-        <v>-3.2085221738e-06</v>
+        <v>-8.1586853441e-06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>